<commit_message>
fixed dply issue in Tourism goal trend calculations and updated documentation of OHI tourism
</commit_message>
<xml_diff>
--- a/prep/tables for documentation.xlsx
+++ b/prep/tables for documentation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Goal</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>average wage</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,6 +531,53 @@
       </c>
       <c r="E9" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>62.5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>65.2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>59.1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>-0.38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>62.4</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-0.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ao goal, layers updated, goal model modified. need additional information on beach access by region and total biomass by island
</commit_message>
<xml_diff>
--- a/prep/tables for documentation.xlsx
+++ b/prep/tables for documentation.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -447,7 +447,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1">
@@ -460,7 +460,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1">
@@ -473,7 +473,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
@@ -486,7 +486,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -511,7 +511,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3">
         <v>4</v>
       </c>

</xml_diff>